<commit_message>
Enhancements & fixing bugs
</commit_message>
<xml_diff>
--- a/free_courses_25052024.xlsx
+++ b/free_courses_25052024.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="55">
   <si>
     <t>Course Title</t>
   </si>
@@ -28,19 +28,25 @@
     <t>Release Time</t>
   </si>
   <si>
+    <t>AZ-900 Azure Fundamentals - Microsoft Azure Fundamentals</t>
+  </si>
+  <si>
+    <t>Web Applications Step by Step Guide Part - 3</t>
+  </si>
+  <si>
+    <t>Web Application: Step by Step Guide</t>
+  </si>
+  <si>
+    <t>Web Applications Step by Step Guide Part-2</t>
+  </si>
+  <si>
+    <t>Web Applications Step by Step Guide Part 4</t>
+  </si>
+  <si>
     <t>18 Crucial Cyber Security Tips</t>
   </si>
   <si>
-    <t>Web Applications Step by Step Guide Part-2</t>
-  </si>
-  <si>
-    <t>Web Applications Step by Step Guide Part 4</t>
-  </si>
-  <si>
-    <t>Web Applications Step by Step Guide Part - 3</t>
-  </si>
-  <si>
-    <t>Web Application: Step by Step Guide</t>
+    <t>Linux Mastery: CLI &amp; Kali Commands Practice Tests 2024 pro</t>
   </si>
   <si>
     <t>Exam MS-900: Microsoft 365 Fundamentals Mock Exams</t>
@@ -49,36 +55,30 @@
     <t>Learn Embarcadero Borland C++ Builder in 1 hour</t>
   </si>
   <si>
-    <t>Linux Mastery: CLI &amp; Kali Commands Practice Tests 2024 pro</t>
+    <t>CompTIA Security+ (SY0-701) Practice Tests</t>
+  </si>
+  <si>
+    <t>(ISC)2 Certified in Cybersecurity (CC) Practice Exams</t>
   </si>
   <si>
     <t>(ISC)2 Certified in Cybersecurity (CC) Practice Exams: Set 2</t>
   </si>
   <si>
-    <t>(ISC)2 Certified in Cybersecurity (CC) Practice Exams</t>
-  </si>
-  <si>
     <t>PCEP (30-02) Practice Exams</t>
   </si>
   <si>
-    <t>CompTIA Security+ (SY0-701) Practice Tests</t>
-  </si>
-  <si>
     <t>CSS And Javascript Crash Course</t>
   </si>
   <si>
-    <t>AZ-900 Azure Fundamentals - Microsoft Azure Fundamentals</t>
-  </si>
-  <si>
-    <t>MS-900: Microsoft 365 Fundamentals Practice Questions 2024</t>
+    <t>ECCouncil: Certified Cybersecurity Technician</t>
+  </si>
+  <si>
+    <t>Web Automation and Scraping using Python</t>
   </si>
   <si>
     <t>The Best ChatGPT &amp; AI Course: Make Money With AI</t>
   </si>
   <si>
-    <t>Web Automation and Scraping using Python</t>
-  </si>
-  <si>
     <t>Learn Azure Bicep</t>
   </si>
   <si>
@@ -88,28 +88,34 @@
     <t>Google Forms o Formularios de Cero a Avanzado</t>
   </si>
   <si>
+    <t>IT &amp; Software &gt; IT Certifications</t>
+  </si>
+  <si>
+    <t>IT &amp; Software &gt; Other IT &amp; Software</t>
+  </si>
+  <si>
     <t>IT &amp; Software &gt; Network &amp; Security</t>
   </si>
   <si>
-    <t>IT &amp; Software &gt; Other IT &amp; Software</t>
-  </si>
-  <si>
-    <t>IT &amp; Software &gt; IT Certifications</t>
+    <t>https://www.real.discount/offer/az-900-azure-fundamentals-microsoft-azure-fundamentals-15711</t>
+  </si>
+  <si>
+    <t>https://www.real.discount/offer/web-applications-step-by-step-guide-part-3-27522</t>
+  </si>
+  <si>
+    <t>https://www.real.discount/offer/web-application-step-by-step-guide-27524</t>
+  </si>
+  <si>
+    <t>https://www.real.discount/offer/web-applications-step-by-step-guide-part-2-27523</t>
+  </si>
+  <si>
+    <t>https://www.real.discount/offer/web-applications-step-by-step-guide-part-4-27521</t>
   </si>
   <si>
     <t>https://www.real.discount/offer/18-crucial-cyber-security-tips-29894</t>
   </si>
   <si>
-    <t>https://www.real.discount/offer/web-applications-step-by-step-guide-part-2-27523</t>
-  </si>
-  <si>
-    <t>https://www.real.discount/offer/web-applications-step-by-step-guide-part-4-27521</t>
-  </si>
-  <si>
-    <t>https://www.real.discount/offer/web-applications-step-by-step-guide-part-3-27522</t>
-  </si>
-  <si>
-    <t>https://www.real.discount/offer/web-application-step-by-step-guide-27524</t>
+    <t>https://www.real.discount/offer/linux-mastery-cli-kali-commands-practice-tests-2024-pro-38400</t>
   </si>
   <si>
     <t>https://www.real.discount/offer/exam-ms-900-microsoft-365-fundamentals-mock-exams-35283</t>
@@ -118,36 +124,30 @@
     <t>https://www.real.discount/offer/learn-embarcadero-borland-c-builder-in-1-hour-2</t>
   </si>
   <si>
-    <t>https://www.real.discount/offer/linux-mastery-cli-kali-commands-practice-tests-2024-pro-38400</t>
+    <t>https://www.real.discount/offer/comptia-security-sy0-701-practice-tests-36461</t>
+  </si>
+  <si>
+    <t>https://www.real.discount/offer/isc-2-certified-in-cybersecurity-cc-practice-exams-36420</t>
   </si>
   <si>
     <t>https://www.real.discount/offer/isc-2-certified-in-cybersecurity-cc-practice-exams-set-2-36444</t>
   </si>
   <si>
-    <t>https://www.real.discount/offer/isc-2-certified-in-cybersecurity-cc-practice-exams-36420</t>
-  </si>
-  <si>
     <t>https://www.real.discount/offer/pcep-30-02-practice-exams-36925</t>
   </si>
   <si>
-    <t>https://www.real.discount/offer/comptia-security-sy0-701-practice-tests-36461</t>
-  </si>
-  <si>
     <t>https://www.real.discount/offer/css-and-javascript-crash-course-13022</t>
   </si>
   <si>
-    <t>https://www.real.discount/offer/az-900-azure-fundamentals-microsoft-azure-fundamentals-15711</t>
-  </si>
-  <si>
-    <t>https://www.real.discount/offer/ms-900-microsoft-365-fundamentals-practice-questions-2024-39190</t>
+    <t>https://www.real.discount/offer/eccouncil-certified-cybersecurity-technician-39209</t>
+  </si>
+  <si>
+    <t>https://www.real.discount/offer/web-automation-and-scraping-using-python-36771</t>
   </si>
   <si>
     <t>https://www.real.discount/offer/the-best-chatgpt-ai-course-make-money-with-ai-35563</t>
   </si>
   <si>
-    <t>https://www.real.discount/offer/web-automation-and-scraping-using-python-36771</t>
-  </si>
-  <si>
     <t>https://www.real.discount/offer/learn-azure-bicep-20512</t>
   </si>
   <si>
@@ -157,6 +157,9 @@
     <t>https://www.real.discount/offer/google-forms-o-formularios-de-cero-a-avanzado-32061</t>
   </si>
   <si>
+    <t>an hour ago</t>
+  </si>
+  <si>
     <t>9 hours ago</t>
   </si>
   <si>
@@ -169,19 +172,13 @@
     <t>4 hours ago</t>
   </si>
   <si>
-    <t>36 minutes ago</t>
-  </si>
-  <si>
-    <t>13 hours ago</t>
+    <t>3 minutes ago</t>
   </si>
   <si>
     <t>12 hours ago</t>
   </si>
   <si>
     <t>11 hours ago</t>
-  </si>
-  <si>
-    <t>10 hours ago</t>
   </si>
 </sst>
 </file>
@@ -552,7 +549,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D31"/>
+  <dimension ref="A1:D21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -603,7 +600,7 @@
         <v>28</v>
       </c>
       <c r="D3" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
     </row>
     <row r="4" spans="1:4">
@@ -617,7 +614,7 @@
         <v>29</v>
       </c>
       <c r="D4" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
     </row>
     <row r="5" spans="1:4">
@@ -631,371 +628,231 @@
         <v>30</v>
       </c>
       <c r="D5" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
     </row>
     <row r="6" spans="1:4">
       <c r="A6" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B6" t="s">
         <v>25</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="D6" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
     </row>
     <row r="7" spans="1:4">
       <c r="A7" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B7" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="D7" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
     </row>
     <row r="8" spans="1:4">
       <c r="A8" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B8" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="D8" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
     </row>
     <row r="9" spans="1:4">
       <c r="A9" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B9" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="D9" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
     </row>
     <row r="10" spans="1:4">
       <c r="A10" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="B10" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="D10" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
     </row>
     <row r="11" spans="1:4">
       <c r="A11" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="B11" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="D11" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
     </row>
     <row r="12" spans="1:4">
       <c r="A12" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="B12" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="D12" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
     </row>
     <row r="13" spans="1:4">
       <c r="A13" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="B13" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="D13" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
     </row>
     <row r="14" spans="1:4">
       <c r="A14" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="B14" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="D14" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
     </row>
     <row r="15" spans="1:4">
       <c r="A15" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="B15" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="D15" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
     </row>
     <row r="16" spans="1:4">
       <c r="A16" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="B16" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="D16" t="s">
-        <v>49</v>
+        <v>52</v>
       </c>
     </row>
     <row r="17" spans="1:4">
       <c r="A17" t="s">
-        <v>12</v>
+        <v>19</v>
       </c>
       <c r="B17" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>35</v>
+        <v>42</v>
       </c>
       <c r="D17" t="s">
-        <v>49</v>
+        <v>53</v>
       </c>
     </row>
     <row r="18" spans="1:4">
       <c r="A18" t="s">
-        <v>13</v>
+        <v>20</v>
       </c>
       <c r="B18" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>36</v>
+        <v>43</v>
       </c>
       <c r="D18" t="s">
-        <v>49</v>
+        <v>53</v>
       </c>
     </row>
     <row r="19" spans="1:4">
       <c r="A19" t="s">
-        <v>11</v>
+        <v>21</v>
       </c>
       <c r="B19" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>34</v>
+        <v>44</v>
       </c>
       <c r="D19" t="s">
-        <v>49</v>
+        <v>54</v>
       </c>
     </row>
     <row r="20" spans="1:4">
       <c r="A20" t="s">
-        <v>14</v>
+        <v>22</v>
       </c>
       <c r="B20" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>37</v>
+        <v>45</v>
       </c>
       <c r="D20" t="s">
-        <v>49</v>
+        <v>54</v>
       </c>
     </row>
     <row r="21" spans="1:4">
       <c r="A21" t="s">
-        <v>15</v>
+        <v>23</v>
       </c>
       <c r="B21" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>38</v>
+        <v>46</v>
       </c>
       <c r="D21" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4">
-      <c r="A22" t="s">
-        <v>16</v>
-      </c>
-      <c r="B22" t="s">
-        <v>26</v>
-      </c>
-      <c r="C22" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="D22" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4">
-      <c r="A23" t="s">
-        <v>16</v>
-      </c>
-      <c r="B23" t="s">
-        <v>26</v>
-      </c>
-      <c r="C23" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="D23" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4">
-      <c r="A24" t="s">
-        <v>17</v>
-      </c>
-      <c r="B24" t="s">
-        <v>26</v>
-      </c>
-      <c r="C24" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="D24" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4">
-      <c r="A25" t="s">
-        <v>17</v>
-      </c>
-      <c r="B25" t="s">
-        <v>26</v>
-      </c>
-      <c r="C25" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="D25" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4">
-      <c r="A26" t="s">
-        <v>18</v>
-      </c>
-      <c r="B26" t="s">
-        <v>26</v>
-      </c>
-      <c r="C26" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="D26" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4">
-      <c r="A27" t="s">
-        <v>19</v>
-      </c>
-      <c r="B27" t="s">
-        <v>25</v>
-      </c>
-      <c r="C27" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="D27" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4">
-      <c r="A28" t="s">
-        <v>20</v>
-      </c>
-      <c r="B28" t="s">
-        <v>25</v>
-      </c>
-      <c r="C28" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="D28" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4">
-      <c r="A29" t="s">
-        <v>21</v>
-      </c>
-      <c r="B29" t="s">
-        <v>25</v>
-      </c>
-      <c r="C29" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="D29" t="s">
         <v>54</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4">
-      <c r="A30" t="s">
-        <v>22</v>
-      </c>
-      <c r="B30" t="s">
-        <v>25</v>
-      </c>
-      <c r="C30" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="D30" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4">
-      <c r="A31" t="s">
-        <v>23</v>
-      </c>
-      <c r="B31" t="s">
-        <v>25</v>
-      </c>
-      <c r="C31" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="D31" t="s">
-        <v>55</v>
       </c>
     </row>
   </sheetData>
@@ -1020,16 +877,6 @@
     <hyperlink ref="C19" r:id="rId18"/>
     <hyperlink ref="C20" r:id="rId19"/>
     <hyperlink ref="C21" r:id="rId20"/>
-    <hyperlink ref="C22" r:id="rId21"/>
-    <hyperlink ref="C23" r:id="rId22"/>
-    <hyperlink ref="C24" r:id="rId23"/>
-    <hyperlink ref="C25" r:id="rId24"/>
-    <hyperlink ref="C26" r:id="rId25"/>
-    <hyperlink ref="C27" r:id="rId26"/>
-    <hyperlink ref="C28" r:id="rId27"/>
-    <hyperlink ref="C29" r:id="rId28"/>
-    <hyperlink ref="C30" r:id="rId29"/>
-    <hyperlink ref="C31" r:id="rId30"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Saving user preferences feature
</commit_message>
<xml_diff>
--- a/free_courses_25052024.xlsx
+++ b/free_courses_25052024.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="57">
   <si>
     <t>Course Title</t>
   </si>
@@ -28,157 +28,163 @@
     <t>Release Time</t>
   </si>
   <si>
+    <t>Learn Embarcadero Borland C++ Builder in 1 hour</t>
+  </si>
+  <si>
+    <t>Exam MS-900: Microsoft 365 Fundamentals Mock Exams</t>
+  </si>
+  <si>
+    <t>PCEP (30-02) Practice Exams</t>
+  </si>
+  <si>
+    <t>Linux Mastery: CLI &amp; Kali Commands Practice Tests 2024 pro</t>
+  </si>
+  <si>
+    <t>(ISC)2 Certified in Cybersecurity (CC) Practice Exams</t>
+  </si>
+  <si>
+    <t>(ISC)2 Certified in Cybersecurity (CC) Practice Exams: Set 2</t>
+  </si>
+  <si>
+    <t>CompTIA Security+ (SY0-701) Practice Tests</t>
+  </si>
+  <si>
+    <t>CSS And Javascript Crash Course</t>
+  </si>
+  <si>
+    <t>ECCouncil: Certified Cybersecurity Technician</t>
+  </si>
+  <si>
     <t>AZ-900 Azure Fundamentals - Microsoft Azure Fundamentals</t>
   </si>
   <si>
+    <t>Salesforce Certified Platform Developer I 2023</t>
+  </si>
+  <si>
+    <t>The Best ChatGPT &amp; AI Course: Make Money With AI</t>
+  </si>
+  <si>
+    <t>Midjourney for Beginners: Embark on Your Artistic Journey</t>
+  </si>
+  <si>
+    <t>Learn Azure Bicep</t>
+  </si>
+  <si>
+    <t>Google Forms o Formularios de Cero a Avanzado</t>
+  </si>
+  <si>
+    <t>18 Crucial Cyber Security Tips</t>
+  </si>
+  <si>
+    <t>Web Applications Step by Step Guide Part 4</t>
+  </si>
+  <si>
+    <t>Web Applications Step by Step Guide Part-2</t>
+  </si>
+  <si>
+    <t>Web Application: Step by Step Guide</t>
+  </si>
+  <si>
     <t>Web Applications Step by Step Guide Part - 3</t>
   </si>
   <si>
-    <t>Web Application: Step by Step Guide</t>
-  </si>
-  <si>
-    <t>Web Applications Step by Step Guide Part-2</t>
-  </si>
-  <si>
-    <t>Web Applications Step by Step Guide Part 4</t>
-  </si>
-  <si>
-    <t>18 Crucial Cyber Security Tips</t>
-  </si>
-  <si>
-    <t>Linux Mastery: CLI &amp; Kali Commands Practice Tests 2024 pro</t>
-  </si>
-  <si>
-    <t>Exam MS-900: Microsoft 365 Fundamentals Mock Exams</t>
-  </si>
-  <si>
-    <t>Learn Embarcadero Borland C++ Builder in 1 hour</t>
-  </si>
-  <si>
-    <t>CompTIA Security+ (SY0-701) Practice Tests</t>
-  </si>
-  <si>
-    <t>(ISC)2 Certified in Cybersecurity (CC) Practice Exams</t>
-  </si>
-  <si>
-    <t>(ISC)2 Certified in Cybersecurity (CC) Practice Exams: Set 2</t>
-  </si>
-  <si>
-    <t>PCEP (30-02) Practice Exams</t>
-  </si>
-  <si>
-    <t>CSS And Javascript Crash Course</t>
-  </si>
-  <si>
-    <t>ECCouncil: Certified Cybersecurity Technician</t>
-  </si>
-  <si>
-    <t>Web Automation and Scraping using Python</t>
-  </si>
-  <si>
-    <t>The Best ChatGPT &amp; AI Course: Make Money With AI</t>
-  </si>
-  <si>
-    <t>Learn Azure Bicep</t>
-  </si>
-  <si>
-    <t>Midjourney for Beginners: Embark on Your Artistic Journey</t>
-  </si>
-  <si>
-    <t>Google Forms o Formularios de Cero a Avanzado</t>
+    <t>IT &amp; Software &gt; Other IT &amp; Software</t>
   </si>
   <si>
     <t>IT &amp; Software &gt; IT Certifications</t>
   </si>
   <si>
-    <t>IT &amp; Software &gt; Other IT &amp; Software</t>
-  </si>
-  <si>
     <t>IT &amp; Software &gt; Network &amp; Security</t>
   </si>
   <si>
+    <t>https://www.real.discount/offer/learn-embarcadero-borland-c-builder-in-1-hour-2</t>
+  </si>
+  <si>
+    <t>https://www.real.discount/offer/exam-ms-900-microsoft-365-fundamentals-mock-exams-35283</t>
+  </si>
+  <si>
+    <t>https://www.real.discount/offer/pcep-30-02-practice-exams-36925</t>
+  </si>
+  <si>
+    <t>https://www.real.discount/offer/linux-mastery-cli-kali-commands-practice-tests-2024-pro-38400</t>
+  </si>
+  <si>
+    <t>https://www.real.discount/offer/isc-2-certified-in-cybersecurity-cc-practice-exams-36420</t>
+  </si>
+  <si>
+    <t>https://www.real.discount/offer/isc-2-certified-in-cybersecurity-cc-practice-exams-set-2-36444</t>
+  </si>
+  <si>
+    <t>https://www.real.discount/offer/comptia-security-sy0-701-practice-tests-36461</t>
+  </si>
+  <si>
+    <t>https://www.real.discount/offer/css-and-javascript-crash-course-13022</t>
+  </si>
+  <si>
+    <t>https://www.real.discount/offer/eccouncil-certified-cybersecurity-technician-39209</t>
+  </si>
+  <si>
     <t>https://www.real.discount/offer/az-900-azure-fundamentals-microsoft-azure-fundamentals-15711</t>
   </si>
   <si>
+    <t>https://www.real.discount/offer/salesforce-certified-platform-developer-i-2023-37805</t>
+  </si>
+  <si>
+    <t>https://www.real.discount/offer/the-best-chatgpt-ai-course-make-money-with-ai-35563</t>
+  </si>
+  <si>
+    <t>https://www.real.discount/offer/midjourney-for-beginners-embark-on-your-artistic-journey-35457</t>
+  </si>
+  <si>
+    <t>https://www.real.discount/offer/learn-azure-bicep-20512</t>
+  </si>
+  <si>
+    <t>https://www.real.discount/offer/google-forms-o-formularios-de-cero-a-avanzado-32061</t>
+  </si>
+  <si>
+    <t>https://www.real.discount/offer/18-crucial-cyber-security-tips-29894</t>
+  </si>
+  <si>
+    <t>https://www.real.discount/offer/web-applications-step-by-step-guide-part-4-27521</t>
+  </si>
+  <si>
+    <t>https://www.real.discount/offer/web-applications-step-by-step-guide-part-2-27523</t>
+  </si>
+  <si>
+    <t>https://www.real.discount/offer/web-application-step-by-step-guide-27524</t>
+  </si>
+  <si>
     <t>https://www.real.discount/offer/web-applications-step-by-step-guide-part-3-27522</t>
   </si>
   <si>
-    <t>https://www.real.discount/offer/web-application-step-by-step-guide-27524</t>
-  </si>
-  <si>
-    <t>https://www.real.discount/offer/web-applications-step-by-step-guide-part-2-27523</t>
-  </si>
-  <si>
-    <t>https://www.real.discount/offer/web-applications-step-by-step-guide-part-4-27521</t>
-  </si>
-  <si>
-    <t>https://www.real.discount/offer/18-crucial-cyber-security-tips-29894</t>
-  </si>
-  <si>
-    <t>https://www.real.discount/offer/linux-mastery-cli-kali-commands-practice-tests-2024-pro-38400</t>
-  </si>
-  <si>
-    <t>https://www.real.discount/offer/exam-ms-900-microsoft-365-fundamentals-mock-exams-35283</t>
-  </si>
-  <si>
-    <t>https://www.real.discount/offer/learn-embarcadero-borland-c-builder-in-1-hour-2</t>
-  </si>
-  <si>
-    <t>https://www.real.discount/offer/comptia-security-sy0-701-practice-tests-36461</t>
-  </si>
-  <si>
-    <t>https://www.real.discount/offer/isc-2-certified-in-cybersecurity-cc-practice-exams-36420</t>
-  </si>
-  <si>
-    <t>https://www.real.discount/offer/isc-2-certified-in-cybersecurity-cc-practice-exams-set-2-36444</t>
-  </si>
-  <si>
-    <t>https://www.real.discount/offer/pcep-30-02-practice-exams-36925</t>
-  </si>
-  <si>
-    <t>https://www.real.discount/offer/css-and-javascript-crash-course-13022</t>
-  </si>
-  <si>
-    <t>https://www.real.discount/offer/eccouncil-certified-cybersecurity-technician-39209</t>
-  </si>
-  <si>
-    <t>https://www.real.discount/offer/web-automation-and-scraping-using-python-36771</t>
-  </si>
-  <si>
-    <t>https://www.real.discount/offer/the-best-chatgpt-ai-course-make-money-with-ai-35563</t>
-  </si>
-  <si>
-    <t>https://www.real.discount/offer/learn-azure-bicep-20512</t>
-  </si>
-  <si>
-    <t>https://www.real.discount/offer/midjourney-for-beginners-embark-on-your-artistic-journey-35457</t>
-  </si>
-  <si>
-    <t>https://www.real.discount/offer/google-forms-o-formularios-de-cero-a-avanzado-32061</t>
-  </si>
-  <si>
-    <t>an hour ago</t>
-  </si>
-  <si>
-    <t>9 hours ago</t>
+    <t>8 hours ago</t>
   </si>
   <si>
     <t>7 hours ago</t>
   </si>
   <si>
-    <t>6 hours ago</t>
-  </si>
-  <si>
-    <t>4 hours ago</t>
-  </si>
-  <si>
-    <t>3 minutes ago</t>
+    <t>5 hours ago</t>
+  </si>
+  <si>
+    <t>29 minutes ago</t>
+  </si>
+  <si>
+    <t>2 hours ago</t>
+  </si>
+  <si>
+    <t>17 minutes ago</t>
+  </si>
+  <si>
+    <t>13 hours ago</t>
   </si>
   <si>
     <t>12 hours ago</t>
   </si>
   <si>
     <t>11 hours ago</t>
+  </si>
+  <si>
+    <t>10 hours ago</t>
   </si>
 </sst>
 </file>
@@ -600,7 +606,7 @@
         <v>28</v>
       </c>
       <c r="D3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="4" spans="1:4">
@@ -650,7 +656,7 @@
         <v>9</v>
       </c>
       <c r="B7" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C7" s="2" t="s">
         <v>32</v>
@@ -664,13 +670,13 @@
         <v>10</v>
       </c>
       <c r="B8" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="C8" s="2" t="s">
         <v>33</v>
       </c>
       <c r="D8" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="9" spans="1:4">
@@ -678,7 +684,7 @@
         <v>11</v>
       </c>
       <c r="B9" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="C9" s="2" t="s">
         <v>34</v>
@@ -698,7 +704,7 @@
         <v>35</v>
       </c>
       <c r="D10" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
     </row>
     <row r="11" spans="1:4">
@@ -706,13 +712,13 @@
         <v>13</v>
       </c>
       <c r="B11" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="C11" s="2" t="s">
         <v>36</v>
       </c>
       <c r="D11" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
     </row>
     <row r="12" spans="1:4">
@@ -720,13 +726,13 @@
         <v>14</v>
       </c>
       <c r="B12" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="C12" s="2" t="s">
         <v>37</v>
       </c>
       <c r="D12" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
     </row>
     <row r="13" spans="1:4">
@@ -740,7 +746,7 @@
         <v>38</v>
       </c>
       <c r="D13" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
     </row>
     <row r="14" spans="1:4">
@@ -754,7 +760,7 @@
         <v>39</v>
       </c>
       <c r="D14" t="s">
-        <v>50</v>
+        <v>54</v>
       </c>
     </row>
     <row r="15" spans="1:4">
@@ -768,7 +774,7 @@
         <v>40</v>
       </c>
       <c r="D15" t="s">
-        <v>51</v>
+        <v>54</v>
       </c>
     </row>
     <row r="16" spans="1:4">
@@ -782,7 +788,7 @@
         <v>41</v>
       </c>
       <c r="D16" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
     </row>
     <row r="17" spans="1:4">
@@ -790,13 +796,13 @@
         <v>19</v>
       </c>
       <c r="B17" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="C17" s="2" t="s">
         <v>42</v>
       </c>
       <c r="D17" t="s">
-        <v>53</v>
+        <v>56</v>
       </c>
     </row>
     <row r="18" spans="1:4">
@@ -804,13 +810,13 @@
         <v>20</v>
       </c>
       <c r="B18" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C18" s="2" t="s">
         <v>43</v>
       </c>
       <c r="D18" t="s">
-        <v>53</v>
+        <v>56</v>
       </c>
     </row>
     <row r="19" spans="1:4">
@@ -818,13 +824,13 @@
         <v>21</v>
       </c>
       <c r="B19" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C19" s="2" t="s">
         <v>44</v>
       </c>
       <c r="D19" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
     </row>
     <row r="20" spans="1:4">
@@ -832,13 +838,13 @@
         <v>22</v>
       </c>
       <c r="B20" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C20" s="2" t="s">
         <v>45</v>
       </c>
       <c r="D20" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
     </row>
     <row r="21" spans="1:4">
@@ -846,13 +852,13 @@
         <v>23</v>
       </c>
       <c r="B21" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C21" s="2" t="s">
         <v>46</v>
       </c>
       <c r="D21" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Adding desktop notifications & fixing GUI
</commit_message>
<xml_diff>
--- a/free_courses_25052024.xlsx
+++ b/free_courses_25052024.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="31">
   <si>
     <t>Course Title</t>
   </si>
@@ -28,7 +28,10 @@
     <t>Release Time</t>
   </si>
   <si>
-    <t>Learn Embarcadero Borland C++ Builder in 1 hour</t>
+    <t>ECCouncil: Certified Cybersecurity Technician</t>
+  </si>
+  <si>
+    <t>Linux Mastery: CLI &amp; Kali Commands Practice Tests 2024 pro</t>
   </si>
   <si>
     <t>Exam MS-900: Microsoft 365 Fundamentals Mock Exams</t>
@@ -37,67 +40,31 @@
     <t>PCEP (30-02) Practice Exams</t>
   </si>
   <si>
-    <t>Linux Mastery: CLI &amp; Kali Commands Practice Tests 2024 pro</t>
+    <t>CompTIA Security+ (SY0-701) Practice Tests</t>
+  </si>
+  <si>
+    <t>(ISC)2 Certified in Cybersecurity (CC) Practice Exams: Set 2</t>
   </si>
   <si>
     <t>(ISC)2 Certified in Cybersecurity (CC) Practice Exams</t>
   </si>
   <si>
-    <t>(ISC)2 Certified in Cybersecurity (CC) Practice Exams: Set 2</t>
-  </si>
-  <si>
-    <t>CompTIA Security+ (SY0-701) Practice Tests</t>
-  </si>
-  <si>
     <t>CSS And Javascript Crash Course</t>
   </si>
   <si>
-    <t>ECCouncil: Certified Cybersecurity Technician</t>
+    <t>Salesforce Certified Platform Developer I 2023</t>
   </si>
   <si>
     <t>AZ-900 Azure Fundamentals - Microsoft Azure Fundamentals</t>
   </si>
   <si>
-    <t>Salesforce Certified Platform Developer I 2023</t>
-  </si>
-  <si>
-    <t>The Best ChatGPT &amp; AI Course: Make Money With AI</t>
-  </si>
-  <si>
-    <t>Midjourney for Beginners: Embark on Your Artistic Journey</t>
-  </si>
-  <si>
-    <t>Learn Azure Bicep</t>
-  </si>
-  <si>
-    <t>Google Forms o Formularios de Cero a Avanzado</t>
-  </si>
-  <si>
-    <t>18 Crucial Cyber Security Tips</t>
-  </si>
-  <si>
-    <t>Web Applications Step by Step Guide Part 4</t>
-  </si>
-  <si>
-    <t>Web Applications Step by Step Guide Part-2</t>
-  </si>
-  <si>
-    <t>Web Application: Step by Step Guide</t>
-  </si>
-  <si>
-    <t>Web Applications Step by Step Guide Part - 3</t>
-  </si>
-  <si>
-    <t>IT &amp; Software &gt; Other IT &amp; Software</t>
-  </si>
-  <si>
     <t>IT &amp; Software &gt; IT Certifications</t>
   </si>
   <si>
-    <t>IT &amp; Software &gt; Network &amp; Security</t>
-  </si>
-  <si>
-    <t>https://www.real.discount/offer/learn-embarcadero-borland-c-builder-in-1-hour-2</t>
+    <t>https://www.real.discount/offer/eccouncil-certified-cybersecurity-technician-39209</t>
+  </si>
+  <si>
+    <t>https://www.real.discount/offer/linux-mastery-cli-kali-commands-practice-tests-2024-pro-38400</t>
   </si>
   <si>
     <t>https://www.real.discount/offer/exam-ms-900-microsoft-365-fundamentals-mock-exams-35283</t>
@@ -106,55 +73,25 @@
     <t>https://www.real.discount/offer/pcep-30-02-practice-exams-36925</t>
   </si>
   <si>
-    <t>https://www.real.discount/offer/linux-mastery-cli-kali-commands-practice-tests-2024-pro-38400</t>
+    <t>https://www.real.discount/offer/comptia-security-sy0-701-practice-tests-36461</t>
+  </si>
+  <si>
+    <t>https://www.real.discount/offer/isc-2-certified-in-cybersecurity-cc-practice-exams-set-2-36444</t>
   </si>
   <si>
     <t>https://www.real.discount/offer/isc-2-certified-in-cybersecurity-cc-practice-exams-36420</t>
   </si>
   <si>
-    <t>https://www.real.discount/offer/isc-2-certified-in-cybersecurity-cc-practice-exams-set-2-36444</t>
-  </si>
-  <si>
-    <t>https://www.real.discount/offer/comptia-security-sy0-701-practice-tests-36461</t>
-  </si>
-  <si>
     <t>https://www.real.discount/offer/css-and-javascript-crash-course-13022</t>
   </si>
   <si>
-    <t>https://www.real.discount/offer/eccouncil-certified-cybersecurity-technician-39209</t>
+    <t>https://www.real.discount/offer/salesforce-certified-platform-developer-i-2023-37805</t>
   </si>
   <si>
     <t>https://www.real.discount/offer/az-900-azure-fundamentals-microsoft-azure-fundamentals-15711</t>
   </si>
   <si>
-    <t>https://www.real.discount/offer/salesforce-certified-platform-developer-i-2023-37805</t>
-  </si>
-  <si>
-    <t>https://www.real.discount/offer/the-best-chatgpt-ai-course-make-money-with-ai-35563</t>
-  </si>
-  <si>
-    <t>https://www.real.discount/offer/midjourney-for-beginners-embark-on-your-artistic-journey-35457</t>
-  </si>
-  <si>
-    <t>https://www.real.discount/offer/learn-azure-bicep-20512</t>
-  </si>
-  <si>
-    <t>https://www.real.discount/offer/google-forms-o-formularios-de-cero-a-avanzado-32061</t>
-  </si>
-  <si>
-    <t>https://www.real.discount/offer/18-crucial-cyber-security-tips-29894</t>
-  </si>
-  <si>
-    <t>https://www.real.discount/offer/web-applications-step-by-step-guide-part-4-27521</t>
-  </si>
-  <si>
-    <t>https://www.real.discount/offer/web-applications-step-by-step-guide-part-2-27523</t>
-  </si>
-  <si>
-    <t>https://www.real.discount/offer/web-application-step-by-step-guide-27524</t>
-  </si>
-  <si>
-    <t>https://www.real.discount/offer/web-applications-step-by-step-guide-part-3-27522</t>
+    <t>an hour ago</t>
   </si>
   <si>
     <t>8 hours ago</t>
@@ -166,25 +103,10 @@
     <t>5 hours ago</t>
   </si>
   <si>
-    <t>29 minutes ago</t>
+    <t>38 minutes ago</t>
   </si>
   <si>
     <t>2 hours ago</t>
-  </si>
-  <si>
-    <t>17 minutes ago</t>
-  </si>
-  <si>
-    <t>13 hours ago</t>
-  </si>
-  <si>
-    <t>12 hours ago</t>
-  </si>
-  <si>
-    <t>11 hours ago</t>
-  </si>
-  <si>
-    <t>10 hours ago</t>
   </si>
 </sst>
 </file>
@@ -555,7 +477,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D21"/>
+  <dimension ref="A1:D11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -586,13 +508,13 @@
         <v>4</v>
       </c>
       <c r="B2" t="s">
-        <v>24</v>
+        <v>14</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>27</v>
+        <v>15</v>
       </c>
       <c r="D2" t="s">
-        <v>47</v>
+        <v>25</v>
       </c>
     </row>
     <row r="3" spans="1:4">
@@ -600,13 +522,13 @@
         <v>5</v>
       </c>
       <c r="B3" t="s">
-        <v>25</v>
+        <v>14</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>28</v>
+        <v>16</v>
       </c>
       <c r="D3" t="s">
-        <v>47</v>
+        <v>26</v>
       </c>
     </row>
     <row r="4" spans="1:4">
@@ -614,13 +536,13 @@
         <v>6</v>
       </c>
       <c r="B4" t="s">
-        <v>25</v>
+        <v>14</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>29</v>
+        <v>17</v>
       </c>
       <c r="D4" t="s">
-        <v>48</v>
+        <v>26</v>
       </c>
     </row>
     <row r="5" spans="1:4">
@@ -628,13 +550,13 @@
         <v>7</v>
       </c>
       <c r="B5" t="s">
-        <v>25</v>
+        <v>14</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>30</v>
+        <v>18</v>
       </c>
       <c r="D5" t="s">
-        <v>48</v>
+        <v>27</v>
       </c>
     </row>
     <row r="6" spans="1:4">
@@ -642,13 +564,13 @@
         <v>8</v>
       </c>
       <c r="B6" t="s">
-        <v>25</v>
+        <v>14</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>31</v>
+        <v>19</v>
       </c>
       <c r="D6" t="s">
-        <v>48</v>
+        <v>27</v>
       </c>
     </row>
     <row r="7" spans="1:4">
@@ -656,13 +578,13 @@
         <v>9</v>
       </c>
       <c r="B7" t="s">
-        <v>25</v>
+        <v>14</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>32</v>
+        <v>20</v>
       </c>
       <c r="D7" t="s">
-        <v>48</v>
+        <v>27</v>
       </c>
     </row>
     <row r="8" spans="1:4">
@@ -670,13 +592,13 @@
         <v>10</v>
       </c>
       <c r="B8" t="s">
-        <v>25</v>
+        <v>14</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>33</v>
+        <v>21</v>
       </c>
       <c r="D8" t="s">
-        <v>48</v>
+        <v>27</v>
       </c>
     </row>
     <row r="9" spans="1:4">
@@ -684,13 +606,13 @@
         <v>11</v>
       </c>
       <c r="B9" t="s">
-        <v>25</v>
+        <v>14</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>34</v>
+        <v>22</v>
       </c>
       <c r="D9" t="s">
-        <v>49</v>
+        <v>28</v>
       </c>
     </row>
     <row r="10" spans="1:4">
@@ -698,13 +620,13 @@
         <v>12</v>
       </c>
       <c r="B10" t="s">
-        <v>25</v>
+        <v>14</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>35</v>
+        <v>23</v>
       </c>
       <c r="D10" t="s">
-        <v>50</v>
+        <v>29</v>
       </c>
     </row>
     <row r="11" spans="1:4">
@@ -712,153 +634,13 @@
         <v>13</v>
       </c>
       <c r="B11" t="s">
-        <v>25</v>
+        <v>14</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>36</v>
+        <v>24</v>
       </c>
       <c r="D11" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4">
-      <c r="A12" t="s">
-        <v>14</v>
-      </c>
-      <c r="B12" t="s">
-        <v>25</v>
-      </c>
-      <c r="C12" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="D12" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4">
-      <c r="A13" t="s">
-        <v>15</v>
-      </c>
-      <c r="B13" t="s">
-        <v>24</v>
-      </c>
-      <c r="C13" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="D13" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4">
-      <c r="A14" t="s">
-        <v>16</v>
-      </c>
-      <c r="B14" t="s">
-        <v>24</v>
-      </c>
-      <c r="C14" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="D14" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4">
-      <c r="A15" t="s">
-        <v>17</v>
-      </c>
-      <c r="B15" t="s">
-        <v>24</v>
-      </c>
-      <c r="C15" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="D15" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4">
-      <c r="A16" t="s">
-        <v>18</v>
-      </c>
-      <c r="B16" t="s">
-        <v>24</v>
-      </c>
-      <c r="C16" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="D16" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4">
-      <c r="A17" t="s">
-        <v>19</v>
-      </c>
-      <c r="B17" t="s">
-        <v>26</v>
-      </c>
-      <c r="C17" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="D17" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4">
-      <c r="A18" t="s">
-        <v>20</v>
-      </c>
-      <c r="B18" t="s">
-        <v>24</v>
-      </c>
-      <c r="C18" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="D18" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4">
-      <c r="A19" t="s">
-        <v>21</v>
-      </c>
-      <c r="B19" t="s">
-        <v>24</v>
-      </c>
-      <c r="C19" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="D19" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4">
-      <c r="A20" t="s">
-        <v>22</v>
-      </c>
-      <c r="B20" t="s">
-        <v>24</v>
-      </c>
-      <c r="C20" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="D20" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4">
-      <c r="A21" t="s">
-        <v>23</v>
-      </c>
-      <c r="B21" t="s">
-        <v>24</v>
-      </c>
-      <c r="C21" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="D21" t="s">
-        <v>56</v>
+        <v>30</v>
       </c>
     </row>
   </sheetData>
@@ -873,16 +655,6 @@
     <hyperlink ref="C9" r:id="rId8"/>
     <hyperlink ref="C10" r:id="rId9"/>
     <hyperlink ref="C11" r:id="rId10"/>
-    <hyperlink ref="C12" r:id="rId11"/>
-    <hyperlink ref="C13" r:id="rId12"/>
-    <hyperlink ref="C14" r:id="rId13"/>
-    <hyperlink ref="C15" r:id="rId14"/>
-    <hyperlink ref="C16" r:id="rId15"/>
-    <hyperlink ref="C17" r:id="rId16"/>
-    <hyperlink ref="C18" r:id="rId17"/>
-    <hyperlink ref="C19" r:id="rId18"/>
-    <hyperlink ref="C20" r:id="rId19"/>
-    <hyperlink ref="C21" r:id="rId20"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>